<commit_message>
Commenting on the refined understanding of of grade based stratification within cNORM, to preserve this understanding for later formal documentation.
</commit_message>
<xml_diff>
--- a/OUTPUT-FILES/NORMS/TODE_8.27.21_fornorms/lske_sum-raw-ss-lookup-tabbed-age.xlsx
+++ b/OUTPUT-FILES/NORMS/TODE_8.27.21_fornorms/lske_sum-raw-ss-lookup-tabbed-age.xlsx
@@ -382,7 +382,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3">
@@ -390,7 +390,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4">
@@ -398,7 +398,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5">
@@ -406,7 +406,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6">
@@ -414,7 +414,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7">
@@ -422,7 +422,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>74</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8">
@@ -430,7 +430,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9">
@@ -438,7 +438,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10">
@@ -446,7 +446,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11">
@@ -454,7 +454,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12">
@@ -462,7 +462,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13">
@@ -470,7 +470,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14">
@@ -478,7 +478,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15">
@@ -486,7 +486,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16">
@@ -494,7 +494,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17">
@@ -502,7 +502,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18">
@@ -510,7 +510,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19">
@@ -518,7 +518,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20">
@@ -526,7 +526,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21">
@@ -534,7 +534,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22">
@@ -542,7 +542,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23">
@@ -550,7 +550,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24">
@@ -558,7 +558,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>121</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25">
@@ -566,7 +566,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>123</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26">
@@ -574,7 +574,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>125</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27">
@@ -582,7 +582,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>128</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28">
@@ -590,7 +590,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>130</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29">
@@ -598,7 +598,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30">
@@ -606,7 +606,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31">
@@ -614,7 +614,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32">
@@ -622,7 +622,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33">
@@ -630,7 +630,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="34">
@@ -671,7 +671,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3">
@@ -679,7 +679,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4">
@@ -687,7 +687,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5">
@@ -695,7 +695,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6">
@@ -703,7 +703,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7">
@@ -711,7 +711,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8">
@@ -719,7 +719,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9">
@@ -727,7 +727,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10">
@@ -735,7 +735,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11">
@@ -743,7 +743,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12">
@@ -751,7 +751,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13">
@@ -759,7 +759,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14">
@@ -767,7 +767,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15">
@@ -775,7 +775,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16">
@@ -783,7 +783,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17">
@@ -791,7 +791,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18">
@@ -799,7 +799,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19">
@@ -807,7 +807,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20">
@@ -815,7 +815,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21">
@@ -823,7 +823,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22">
@@ -831,7 +831,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23">
@@ -839,7 +839,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24">
@@ -847,7 +847,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25">
@@ -855,7 +855,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26">
@@ -863,7 +863,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27">
@@ -871,7 +871,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28">
@@ -879,7 +879,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29">
@@ -887,7 +887,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30">
@@ -895,7 +895,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31">
@@ -903,7 +903,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32">
@@ -911,7 +911,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33">
@@ -960,7 +960,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3">
@@ -968,7 +968,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4">
@@ -976,7 +976,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5">
@@ -1080,7 +1080,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18">
@@ -1104,7 +1104,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21">
@@ -1160,7 +1160,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28">
@@ -1176,7 +1176,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30">
@@ -1184,7 +1184,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31">
@@ -1249,7 +1249,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3">
@@ -1257,7 +1257,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4">
@@ -1265,7 +1265,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5">
@@ -1273,7 +1273,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6">
@@ -1281,7 +1281,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7">
@@ -1289,7 +1289,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8">
@@ -1297,7 +1297,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9">
@@ -1313,7 +1313,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11">
@@ -1321,7 +1321,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12">
@@ -1329,7 +1329,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13">
@@ -1337,7 +1337,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14">
@@ -1353,7 +1353,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16">
@@ -1369,7 +1369,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18">
@@ -1377,7 +1377,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19">
@@ -1385,7 +1385,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20">
@@ -1393,7 +1393,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21">
@@ -1401,7 +1401,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22">
@@ -1409,7 +1409,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23">
@@ -1417,7 +1417,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24">
@@ -1425,7 +1425,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25">
@@ -1433,7 +1433,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26">
@@ -1441,7 +1441,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27">
@@ -1449,7 +1449,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28">
@@ -1457,7 +1457,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29">
@@ -1465,7 +1465,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30">
@@ -1473,7 +1473,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31">
@@ -1481,7 +1481,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32">
@@ -1489,7 +1489,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>121</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33">
@@ -1497,7 +1497,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34">
@@ -1538,7 +1538,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3">
@@ -1546,7 +1546,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4">
@@ -1554,7 +1554,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5">
@@ -1562,7 +1562,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6">
@@ -1586,7 +1586,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9">
@@ -1618,7 +1618,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13">
@@ -1634,7 +1634,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15">
@@ -1650,7 +1650,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17">
@@ -1674,7 +1674,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20">
@@ -1690,7 +1690,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22">
@@ -1698,7 +1698,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23">
@@ -1714,7 +1714,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25">
@@ -1722,7 +1722,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26">
@@ -1730,7 +1730,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27">
@@ -1738,7 +1738,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28">
@@ -1746,7 +1746,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29">
@@ -1754,7 +1754,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30">
@@ -1762,7 +1762,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31">
@@ -1770,7 +1770,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32">
@@ -1778,7 +1778,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33">
@@ -1786,7 +1786,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34">
@@ -1827,7 +1827,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3">
@@ -1835,7 +1835,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4">
@@ -1843,7 +1843,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5">
@@ -1851,7 +1851,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6">
@@ -1875,7 +1875,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9">
@@ -1891,7 +1891,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11">
@@ -1915,7 +1915,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14">
@@ -1939,7 +1939,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17">
@@ -1963,7 +1963,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20">
@@ -1987,7 +1987,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23">
@@ -2003,7 +2003,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25">
@@ -2011,7 +2011,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26">
@@ -2027,7 +2027,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28">
@@ -2035,7 +2035,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29">
@@ -2043,7 +2043,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30">
@@ -2051,7 +2051,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31">
@@ -2059,7 +2059,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32">
@@ -2067,7 +2067,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33">
@@ -2075,7 +2075,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34">
@@ -2083,7 +2083,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2116,7 +2116,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3">
@@ -2124,7 +2124,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4">
@@ -2164,7 +2164,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9">
@@ -2188,7 +2188,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12">
@@ -2220,7 +2220,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16">
@@ -2228,7 +2228,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17">
@@ -2252,7 +2252,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20">
@@ -2260,7 +2260,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21">
@@ -2276,7 +2276,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23">
@@ -2284,7 +2284,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24">
@@ -2300,7 +2300,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26">
@@ -2316,7 +2316,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28">
@@ -2324,7 +2324,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29">
@@ -2332,7 +2332,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30">
@@ -2340,7 +2340,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31">
@@ -2348,7 +2348,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32">
@@ -2356,7 +2356,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33">
@@ -2364,7 +2364,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34">
@@ -2372,7 +2372,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>117</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -2405,7 +2405,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3">
@@ -2413,7 +2413,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4">
@@ -2421,7 +2421,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5">
@@ -2429,7 +2429,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6">
@@ -2437,7 +2437,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7">
@@ -2453,7 +2453,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9">
@@ -2461,7 +2461,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10">
@@ -2485,7 +2485,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13">
@@ -2493,7 +2493,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14">
@@ -2501,7 +2501,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15">
@@ -2509,7 +2509,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16">
@@ -2533,7 +2533,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19">
@@ -2541,7 +2541,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20">
@@ -2549,7 +2549,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21">
@@ -2565,7 +2565,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23">
@@ -2573,7 +2573,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24">
@@ -2581,7 +2581,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25">
@@ -2589,7 +2589,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26">
@@ -2597,7 +2597,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27">
@@ -2605,7 +2605,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28">
@@ -2613,7 +2613,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29">
@@ -2621,7 +2621,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30">
@@ -2629,7 +2629,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31">
@@ -2637,7 +2637,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32">
@@ -2645,7 +2645,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33">
@@ -2653,7 +2653,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>97</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34">
@@ -2661,7 +2661,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>110</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2694,7 +2694,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3">
@@ -2702,7 +2702,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4">
@@ -2710,7 +2710,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5">
@@ -2718,7 +2718,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6">
@@ -2726,7 +2726,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7">
@@ -2734,7 +2734,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8">
@@ -2742,7 +2742,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9">
@@ -2750,7 +2750,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10">
@@ -2758,7 +2758,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11">
@@ -2766,7 +2766,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12">
@@ -2774,7 +2774,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13">
@@ -2782,7 +2782,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14">
@@ -2790,7 +2790,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15">
@@ -2798,7 +2798,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16">
@@ -2806,7 +2806,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17">
@@ -2814,7 +2814,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>62</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18">
@@ -2822,7 +2822,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19">
@@ -2830,7 +2830,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20">
@@ -2838,7 +2838,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21">
@@ -2846,7 +2846,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>66</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22">
@@ -2854,7 +2854,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>67</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23">
@@ -2862,7 +2862,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>69</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24">
@@ -2870,7 +2870,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>70</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25">
@@ -2878,7 +2878,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>71</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26">
@@ -2886,7 +2886,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>73</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27">
@@ -2894,7 +2894,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>74</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28">
@@ -2902,7 +2902,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>76</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29">
@@ -2910,7 +2910,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>77</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30">
@@ -2918,7 +2918,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>79</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31">
@@ -2926,7 +2926,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>82</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32">
@@ -2934,7 +2934,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>85</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33">
@@ -2942,7 +2942,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>90</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34">
@@ -2950,7 +2950,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finish re-run of TODE age norms
</commit_message>
<xml_diff>
--- a/OUTPUT-FILES/NORMS/TODE_8.27.21_fornorms/lske_sum-raw-ss-lookup-tabbed-age.xlsx
+++ b/OUTPUT-FILES/NORMS/TODE_8.27.21_fornorms/lske_sum-raw-ss-lookup-tabbed-age.xlsx
@@ -359,7 +359,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -379,265 +379,273 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>100</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>101</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>105</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>106</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>108</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>109</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>111</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>113</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>115</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>116</v>
+        <v>125</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>118</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>120</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
-        <v>122</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31">
-        <v>124</v>
+        <v>130</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
         <v>33</v>
       </c>
-      <c r="B34">
+      <c r="B35">
         <v>130</v>
       </c>
     </row>
@@ -648,7 +656,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -668,47 +676,47 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>80</v>
@@ -716,7 +724,7 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>82</v>
@@ -724,7 +732,7 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>84</v>
@@ -732,7 +740,7 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>86</v>
@@ -740,7 +748,7 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>88</v>
@@ -748,15 +756,15 @@
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>91</v>
@@ -764,7 +772,7 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>93</v>
@@ -772,23 +780,23 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>98</v>
@@ -796,31 +804,31 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>105</v>
@@ -828,95 +836,95 @@
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33">
         <v>130</v>
@@ -924,9 +932,17 @@
     </row>
     <row r="34">
       <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
         <v>33</v>
       </c>
-      <c r="B34">
+      <c r="B35">
         <v>130</v>
       </c>
     </row>
@@ -937,7 +953,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -957,255 +973,255 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33">
         <v>130</v>
@@ -1213,9 +1229,17 @@
     </row>
     <row r="34">
       <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
         <v>33</v>
       </c>
-      <c r="B34">
+      <c r="B35">
         <v>130</v>
       </c>
     </row>
@@ -1226,7 +1250,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1246,265 +1270,273 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32">
-        <v>128</v>
+        <v>117</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
         <v>33</v>
       </c>
-      <c r="B34">
+      <c r="B35">
         <v>130</v>
       </c>
     </row>
@@ -1515,7 +1547,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1535,265 +1567,273 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
         <v>33</v>
       </c>
-      <c r="B34">
+      <c r="B35">
         <v>130</v>
       </c>
     </row>
@@ -1804,7 +1844,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1824,266 +1864,274 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
         <v>33</v>
       </c>
-      <c r="B34">
-        <v>112</v>
+      <c r="B35">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2093,7 +2141,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2113,119 +2161,119 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>69</v>
@@ -2233,31 +2281,31 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>74</v>
@@ -2265,23 +2313,23 @@
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>78</v>
@@ -2289,90 +2337,98 @@
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
         <v>33</v>
       </c>
-      <c r="B34">
-        <v>104</v>
+      <c r="B35">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -2382,7 +2438,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2402,266 +2458,274 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32">
-        <v>97</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33">
-        <v>116</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
         <v>33</v>
       </c>
-      <c r="B34">
-        <v>121</v>
+      <c r="B35">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2671,7 +2735,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2691,266 +2755,274 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>104</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>104</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>104</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>104</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>104</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>104</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>104</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
-        <v>104</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31">
-        <v>104</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32">
-        <v>104</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33">
-        <v>104</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
         <v>33</v>
       </c>
-      <c r="B34">
-        <v>104</v>
+      <c r="B35">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>